<commit_message>
Added the code that gets the data from Excel
</commit_message>
<xml_diff>
--- a/vendor.xlsx
+++ b/vendor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/saisanthoshkonduri/PycharmProjects/EmailAutomation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3919C5E-44E5-0C41-9DD1-9C0CF58E87D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7569CDAC-3282-264D-BDB0-0FE4BFAC77E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19400" xr2:uid="{D22C5766-FC84-C747-AC7D-9785DF207C04}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>FirstName</t>
   </si>
@@ -45,16 +45,48 @@
   </si>
   <si>
     <t>Email</t>
+  </si>
+  <si>
+    <t>Sandeep</t>
+  </si>
+  <si>
+    <t>konduri</t>
+  </si>
+  <si>
+    <t>sandeep.konduri123@gmail.com</t>
+  </si>
+  <si>
+    <t>santhosh</t>
+  </si>
+  <si>
+    <t>konduri.santhosh96@gmail.com</t>
+  </si>
+  <si>
+    <t>goutham</t>
+  </si>
+  <si>
+    <t>goutham221997@gmail.com</t>
+  </si>
+  <si>
+    <t>vamsi.gch@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -77,13 +109,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -396,13 +431,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88F85C26-B978-3C4D-9E39-E11228CABB85}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="28.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -415,7 +453,46 @@
         <v>2</v>
       </c>
     </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C5" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{E1D81F34-67B5-4F4F-ACE4-BD75B8326B99}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{11F2E2FE-F7B3-1F4F-B9A1-07966F33D841}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Modified the message body
</commit_message>
<xml_diff>
--- a/vendor.xlsx
+++ b/vendor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/saisanthoshkonduri/PycharmProjects/EmailAutomation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7569CDAC-3282-264D-BDB0-0FE4BFAC77E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88D2FE89-067E-F447-B677-28D3CECE220E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19400" xr2:uid="{D22C5766-FC84-C747-AC7D-9785DF207C04}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>FirstName</t>
   </si>
@@ -50,25 +50,28 @@
     <t>Sandeep</t>
   </si>
   <si>
-    <t>konduri</t>
-  </si>
-  <si>
     <t>sandeep.konduri123@gmail.com</t>
   </si>
   <si>
-    <t>santhosh</t>
-  </si>
-  <si>
     <t>konduri.santhosh96@gmail.com</t>
   </si>
   <si>
-    <t>goutham</t>
-  </si>
-  <si>
-    <t>goutham221997@gmail.com</t>
-  </si>
-  <si>
     <t>vamsi.gch@gmail.com</t>
+  </si>
+  <si>
+    <t>Santhosh</t>
+  </si>
+  <si>
+    <t>Konduri</t>
+  </si>
+  <si>
+    <t>Gurijala</t>
+  </si>
+  <si>
+    <t>gurijala2018@gmail.com</t>
+  </si>
+  <si>
+    <t>Vamsi</t>
   </si>
 </sst>
 </file>
@@ -458,32 +461,35 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>8</v>
+      <c r="B4" t="s">
+        <v>9</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
       <c r="C5" s="1" t="s">
         <v>10</v>
       </c>
@@ -492,6 +498,7 @@
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{E1D81F34-67B5-4F4F-ACE4-BD75B8326B99}"/>
     <hyperlink ref="C3" r:id="rId2" xr:uid="{11F2E2FE-F7B3-1F4F-B9A1-07966F33D841}"/>
+    <hyperlink ref="C5" r:id="rId3" xr:uid="{36242801-A268-9A40-B793-9DA075A9A3BF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>